<commit_message>
add twitter scrape code
</commit_message>
<xml_diff>
--- a/schedule_685.xlsx
+++ b/schedule_685.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11014"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\math_685\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rdonatello/GitHub/math_685/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C07DB21F-41ED-4771-9137-2567512AD9BA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{155C46DC-994C-9844-A9E1-717C44741B75}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2080" yWindow="460" windowWidth="36280" windowHeight="19040" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Weekly Detail" sheetId="5" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="83">
   <si>
     <t>Finals Week</t>
   </si>
@@ -1068,24 +1068,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:J29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="51" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" zoomScale="159" zoomScaleNormal="51" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C16" sqref="C16:C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.125" style="3" customWidth="1"/>
-    <col min="2" max="2" width="6.625" style="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.625" style="3" customWidth="1"/>
-    <col min="4" max="7" width="36.875" style="4" customWidth="1"/>
-    <col min="8" max="8" width="36.875" style="3" customWidth="1"/>
-    <col min="9" max="9" width="2.875" style="4" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="88.625" style="3" customWidth="1"/>
-    <col min="11" max="16384" width="14.875" style="3"/>
+    <col min="1" max="1" width="7.1640625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="6.6640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.6640625" style="3" customWidth="1"/>
+    <col min="4" max="5" width="36.83203125" style="4" customWidth="1"/>
+    <col min="6" max="6" width="20" style="4" customWidth="1"/>
+    <col min="7" max="7" width="36.83203125" style="4" customWidth="1"/>
+    <col min="8" max="8" width="36.83203125" style="3" customWidth="1"/>
+    <col min="9" max="9" width="2.83203125" style="4" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="88.6640625" style="3" customWidth="1"/>
+    <col min="11" max="16384" width="14.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="32" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
         <v>1</v>
       </c>
@@ -1114,7 +1116,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="195" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="208" x14ac:dyDescent="0.2">
       <c r="A2" s="12">
         <v>1</v>
       </c>
@@ -1144,7 +1146,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" ht="80" x14ac:dyDescent="0.2">
       <c r="A3" s="12">
         <v>2</v>
       </c>
@@ -1173,7 +1175,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="64" x14ac:dyDescent="0.2">
       <c r="A4" s="12">
         <v>3</v>
       </c>
@@ -1199,7 +1201,7 @@
       </c>
       <c r="I4" s="1"/>
     </row>
-    <row r="5" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" ht="80" x14ac:dyDescent="0.2">
       <c r="A5" s="12">
         <v>4</v>
       </c>
@@ -1225,7 +1227,7 @@
       </c>
       <c r="I5" s="1"/>
     </row>
-    <row r="6" spans="1:10" ht="240" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" ht="256" x14ac:dyDescent="0.2">
       <c r="A6" s="12">
         <v>5</v>
       </c>
@@ -1256,7 +1258,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="12">
         <v>6</v>
       </c>
@@ -1272,7 +1274,7 @@
       <c r="H7" s="14"/>
       <c r="I7" s="1"/>
     </row>
-    <row r="8" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" ht="64" x14ac:dyDescent="0.2">
       <c r="A8" s="12">
         <v>7</v>
       </c>
@@ -1296,7 +1298,7 @@
       <c r="H8" s="14"/>
       <c r="I8" s="1"/>
     </row>
-    <row r="9" spans="1:10" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="12">
         <v>8</v>
       </c>
@@ -1314,7 +1316,7 @@
       </c>
       <c r="I9" s="1"/>
     </row>
-    <row r="10" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" ht="64" x14ac:dyDescent="0.2">
       <c r="A10" s="12">
         <v>9</v>
       </c>
@@ -1338,7 +1340,7 @@
       <c r="H10" s="19"/>
       <c r="I10" s="1"/>
     </row>
-    <row r="11" spans="1:10" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="18">
         <v>10</v>
       </c>
@@ -1360,7 +1362,7 @@
       </c>
       <c r="I11" s="1"/>
     </row>
-    <row r="12" spans="1:10" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" ht="29" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="18">
         <v>11</v>
       </c>
@@ -1380,7 +1382,7 @@
       <c r="H12" s="19"/>
       <c r="I12" s="1"/>
     </row>
-    <row r="13" spans="1:10" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" ht="29" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="18">
         <v>12</v>
       </c>
@@ -1398,7 +1400,7 @@
       </c>
       <c r="I13" s="1"/>
     </row>
-    <row r="14" spans="1:10" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" ht="29" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="18">
         <v>13</v>
       </c>
@@ -1416,7 +1418,7 @@
       <c r="H14" s="19"/>
       <c r="I14" s="1"/>
     </row>
-    <row r="15" spans="1:10" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" ht="29" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="18"/>
       <c r="B15" s="13">
         <f t="shared" si="0"/>
@@ -1430,7 +1432,7 @@
       <c r="H15" s="22"/>
       <c r="I15" s="6"/>
     </row>
-    <row r="16" spans="1:10" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" ht="39" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="18">
         <v>14</v>
       </c>
@@ -1450,7 +1452,7 @@
       <c r="H16" s="19"/>
       <c r="I16" s="1"/>
     </row>
-    <row r="17" spans="1:9" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" ht="29" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="18">
         <v>15</v>
       </c>
@@ -1470,7 +1472,7 @@
       <c r="H17" s="19"/>
       <c r="I17" s="1"/>
     </row>
-    <row r="18" spans="1:9" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" ht="29" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="18" t="s">
         <v>0</v>
       </c>
@@ -1486,7 +1488,7 @@
       <c r="H18" s="19"/>
       <c r="I18" s="1"/>
     </row>
-    <row r="19" spans="1:9" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" ht="29" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="19"/>
       <c r="B19" s="23"/>
       <c r="C19" s="14" t="s">
@@ -1500,7 +1502,7 @@
       <c r="G19" s="15"/>
       <c r="H19" s="19"/>
     </row>
-    <row r="20" spans="1:9" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" ht="29" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="19"/>
       <c r="B20" s="23"/>
       <c r="C20" s="14" t="s">
@@ -1512,7 +1514,7 @@
       <c r="G20" s="15"/>
       <c r="H20" s="19"/>
     </row>
-    <row r="21" spans="1:9" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" ht="29" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C21" s="3" t="s">
         <v>45</v>
       </c>
@@ -1520,8 +1522,8 @@
         <v>46</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="29.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="29" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" ht="29" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="29" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="D29" s="25"/>
     </row>
   </sheetData>
@@ -1539,21 +1541,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A793E651-852A-4512-B8D0-B3343307CB94}">
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView zoomScale="226" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.375" style="26" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.33203125" style="26" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9" style="26"/>
     <col min="3" max="3" width="12.5" style="26" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.125" style="27" customWidth="1"/>
-    <col min="5" max="5" width="18.625" style="26" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.1640625" style="27" customWidth="1"/>
+    <col min="5" max="5" width="18.6640625" style="26" bestFit="1" customWidth="1"/>
     <col min="6" max="16384" width="9" style="26"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="26" t="s">
         <v>59</v>
       </c>
@@ -1570,7 +1572,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="51" x14ac:dyDescent="0.2">
       <c r="A2" s="26" t="s">
         <v>68</v>
       </c>
@@ -1587,7 +1589,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="26" t="s">
         <v>68</v>
       </c>
@@ -1601,7 +1603,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="26" t="s">
         <v>69</v>
       </c>
@@ -1615,7 +1617,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="26" t="s">
         <v>69</v>
       </c>
@@ -1626,7 +1628,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="26" t="s">
         <v>75</v>
       </c>
@@ -1637,7 +1639,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="26" t="s">
         <v>75</v>
       </c>
@@ -1648,7 +1650,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="26" t="s">
         <v>75</v>
       </c>

</xml_diff>

<commit_message>
add islr to schedule
</commit_message>
<xml_diff>
--- a/schedule_685.xlsx
+++ b/schedule_685.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11014"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20352"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rdonatello/GitHub/math_685/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\math_685\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1518237B-0B14-9344-B629-0F779539CE3F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F33D99E-6F25-41C1-9EAE-5F8C26128991}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="20060" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="38400" windowHeight="20055" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Weekly Detail" sheetId="5" r:id="rId1"/>
@@ -19,7 +19,7 @@
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Weekly Detail'!$1:$1</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <fileRecoveryPr autoRecover="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="83">
   <si>
     <t>Finals Week</t>
   </si>
@@ -171,31 +171,10 @@
     <t xml:space="preserve">Dissemination to a broader public. </t>
   </si>
   <si>
-    <t>Clustering methods</t>
-  </si>
-  <si>
-    <t xml:space="preserve">knn, decision trees, </t>
-  </si>
-  <si>
-    <t>PCA, FA</t>
-  </si>
-  <si>
-    <t>Predictive modeling</t>
-  </si>
-  <si>
     <t>Bootstrapping</t>
   </si>
   <si>
-    <t>Unsupervised learning / dimension reduction</t>
-  </si>
-  <si>
-    <t xml:space="preserve">lin reg, log reg, decision trees, </t>
-  </si>
-  <si>
     <t>Relational databases</t>
-  </si>
-  <si>
-    <t>Stat 545 Data Analysis 3</t>
   </si>
   <si>
     <t xml:space="preserve">reproducible data exploration on the gapminder data. Rmarkdown file. Pick 2-3 variables to explore using visualizations. NO ANALSYSIS. But story. Tell a story using the gapminder data. </t>
@@ -324,6 +303,26 @@
   </si>
   <si>
     <t xml:space="preserve">Stat 545: Ch 17 (skim), Ch 18 &amp; 19 (Functions part I and II), OR R for Data Science ch 19 https://r4ds.had.co.nz/functions.html </t>
+  </si>
+  <si>
+    <t>Classification methods</t>
+  </si>
+  <si>
+    <t>Kathleen: Write a function to automate grep pattern matches in master log</t>
+  </si>
+  <si>
+    <t>irf out</t>
+  </si>
+  <si>
+    <t xml:space="preserve">How to use models to predict an event, or group an observation will be in? </t>
+  </si>
+  <si>
+    <t>ASCN Ch 11, 
+https://dzone.com/refcardz/machine-learning-predictive
+ISLR ch 2: What is statistical learning (2.1), Assessing model accuracy (2.2)</t>
+  </si>
+  <si>
+    <t>Cross validation</t>
   </si>
 </sst>
 </file>
@@ -431,7 +430,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -454,6 +453,15 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="80">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -537,7 +545,7 @@
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -602,12 +610,6 @@
     <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="79"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -623,6 +625,30 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="79" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="80">
@@ -1046,24 +1072,24 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E14" sqref="E14"/>
+      <selection pane="bottomLeft" activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="14.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.1640625" style="3" customWidth="1"/>
-    <col min="2" max="2" width="6.6640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.6640625" style="3" customWidth="1"/>
-    <col min="4" max="5" width="36.83203125" style="4" customWidth="1"/>
+    <col min="1" max="1" width="7.125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="6.625" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.625" style="3" customWidth="1"/>
+    <col min="4" max="5" width="36.875" style="4" customWidth="1"/>
     <col min="6" max="6" width="20" style="4" customWidth="1"/>
-    <col min="7" max="7" width="36.83203125" style="4" customWidth="1"/>
-    <col min="8" max="8" width="36.83203125" style="3" customWidth="1"/>
-    <col min="9" max="9" width="2.83203125" style="4" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="88.6640625" style="3" customWidth="1"/>
-    <col min="11" max="16384" width="14.83203125" style="3"/>
+    <col min="7" max="7" width="36.875" style="4" customWidth="1"/>
+    <col min="8" max="8" width="36.875" style="3" customWidth="1"/>
+    <col min="9" max="9" width="2.875" style="4" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="88.625" style="3" customWidth="1"/>
+    <col min="11" max="16384" width="14.875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="32" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>1</v>
       </c>
@@ -1092,7 +1118,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="208" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" ht="195" x14ac:dyDescent="0.25">
       <c r="A2" s="12">
         <v>1</v>
       </c>
@@ -1119,10 +1145,10 @@
       </c>
       <c r="I2" s="1"/>
       <c r="J2" s="5" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" ht="80" x14ac:dyDescent="0.2">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A3" s="12">
         <v>2</v>
       </c>
@@ -1144,14 +1170,14 @@
         <v>16</v>
       </c>
       <c r="H3" s="16" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="I3" s="1"/>
       <c r="J3" s="5" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="64" x14ac:dyDescent="0.2">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A4" s="12">
         <v>3</v>
       </c>
@@ -1177,7 +1203,7 @@
       </c>
       <c r="I4" s="1"/>
     </row>
-    <row r="5" spans="1:10" ht="80" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A5" s="12">
         <v>4</v>
       </c>
@@ -1203,7 +1229,7 @@
       </c>
       <c r="I5" s="1"/>
     </row>
-    <row r="6" spans="1:10" ht="256" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" ht="240" x14ac:dyDescent="0.25">
       <c r="A6" s="12">
         <v>5</v>
       </c>
@@ -1221,20 +1247,20 @@
         <v>35</v>
       </c>
       <c r="F6" s="14" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="G6" s="17" t="s">
         <v>29</v>
       </c>
       <c r="H6" s="16" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="I6" s="1"/>
       <c r="J6" s="3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="12">
         <v>6</v>
       </c>
@@ -1250,7 +1276,7 @@
       <c r="H7" s="14"/>
       <c r="I7" s="1"/>
     </row>
-    <row r="8" spans="1:10" ht="64" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A8" s="12">
         <v>7</v>
       </c>
@@ -1274,7 +1300,7 @@
       <c r="H8" s="14"/>
       <c r="I8" s="1"/>
     </row>
-    <row r="9" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="12">
         <v>8</v>
       </c>
@@ -1288,11 +1314,11 @@
       <c r="F9" s="15"/>
       <c r="G9" s="14"/>
       <c r="H9" s="16" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="I9" s="1"/>
     </row>
-    <row r="10" spans="1:10" ht="64" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A10" s="12">
         <v>9</v>
       </c>
@@ -1301,24 +1327,24 @@
         <v>42297</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="D10" s="14" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="E10" s="17" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="F10" s="14"/>
       <c r="G10" s="14" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="H10" s="16" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="I10" s="1"/>
     </row>
-    <row r="11" spans="1:10" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="12">
         <v>10</v>
       </c>
@@ -1327,20 +1353,23 @@
         <v>42304</v>
       </c>
       <c r="C11" s="19" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="D11" s="14"/>
       <c r="E11" s="15" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="F11" s="14"/>
       <c r="G11" s="14"/>
       <c r="H11" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="I11" s="1"/>
+      <c r="J11" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="I11" s="1"/>
-    </row>
-    <row r="12" spans="1:10" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="12" spans="1:10" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="12">
         <v>11</v>
       </c>
@@ -1355,9 +1384,12 @@
       <c r="G12" s="14"/>
       <c r="H12" s="19"/>
       <c r="I12" s="1"/>
-    </row>
-    <row r="13" spans="1:10" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="18">
+      <c r="J12" s="3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="12">
         <v>12</v>
       </c>
       <c r="B13" s="13">
@@ -1365,21 +1397,24 @@
         <v>42318</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="D13" s="14"/>
       <c r="E13" s="14" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="F13" s="20"/>
       <c r="G13" s="20"/>
       <c r="H13" s="16" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="I13" s="1"/>
-    </row>
-    <row r="14" spans="1:10" ht="52" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="18">
+      <c r="J13" s="3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="51.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="12">
         <v>13</v>
       </c>
       <c r="B14" s="13">
@@ -1391,10 +1426,12 @@
       <c r="E14" s="14"/>
       <c r="F14" s="20"/>
       <c r="G14" s="20"/>
-      <c r="H14" s="16"/>
+      <c r="H14" s="16" t="s">
+        <v>78</v>
+      </c>
       <c r="I14" s="1"/>
     </row>
-    <row r="15" spans="1:10" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="18"/>
       <c r="B15" s="13">
         <f t="shared" si="0"/>
@@ -1408,7 +1445,7 @@
       <c r="H15" s="21"/>
       <c r="I15" s="6"/>
     </row>
-    <row r="16" spans="1:10" ht="39" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="18">
         <v>14</v>
       </c>
@@ -1417,18 +1454,20 @@
         <v>42339</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="D16" s="14"/>
+        <v>77</v>
+      </c>
+      <c r="D16" s="14" t="s">
+        <v>80</v>
+      </c>
       <c r="E16" s="14" t="s">
-        <v>40</v>
+        <v>81</v>
       </c>
       <c r="F16" s="14"/>
       <c r="G16" s="14"/>
       <c r="H16" s="19"/>
       <c r="I16" s="1"/>
     </row>
-    <row r="17" spans="1:9" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="18">
         <v>15</v>
       </c>
@@ -1437,18 +1476,16 @@
         <v>42346</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>41</v>
+        <v>82</v>
       </c>
       <c r="D17" s="14"/>
-      <c r="E17" s="14" t="s">
-        <v>44</v>
-      </c>
+      <c r="E17" s="14"/>
       <c r="F17" s="14"/>
       <c r="G17" s="14"/>
       <c r="H17" s="19"/>
       <c r="I17" s="1"/>
     </row>
-    <row r="18" spans="1:9" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="18" t="s">
         <v>0</v>
       </c>
@@ -1464,49 +1501,43 @@
       <c r="H18" s="19"/>
       <c r="I18" s="1"/>
     </row>
-    <row r="19" spans="1:9" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="19"/>
-      <c r="B19" s="22"/>
-      <c r="C19" s="14" t="s">
+    <row r="19" spans="1:9" s="28" customFormat="1" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="31"/>
+      <c r="B19" s="32"/>
+      <c r="C19" s="33"/>
+      <c r="D19" s="34"/>
+      <c r="E19" s="35"/>
+      <c r="F19" s="34"/>
+      <c r="G19" s="34"/>
+      <c r="H19" s="31"/>
+      <c r="I19" s="30"/>
+    </row>
+    <row r="20" spans="1:9" s="28" customFormat="1" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="29"/>
+      <c r="D20" s="30"/>
+      <c r="E20" s="30"/>
+      <c r="F20" s="30"/>
+      <c r="G20" s="30"/>
+      <c r="I20" s="30"/>
+    </row>
+    <row r="21" spans="1:9" ht="29.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="22" spans="1:9" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C22" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C23" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="D19" s="15"/>
-      <c r="E19" s="23" t="s">
-        <v>39</v>
-      </c>
-      <c r="F19" s="15"/>
-      <c r="G19" s="15"/>
-      <c r="H19" s="19"/>
-    </row>
-    <row r="20" spans="1:9" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="19"/>
-      <c r="B20" s="22"/>
-      <c r="D20" s="15"/>
-      <c r="E20" s="15"/>
-      <c r="F20" s="15"/>
-      <c r="G20" s="15"/>
-      <c r="H20" s="19"/>
-    </row>
-    <row r="21" spans="1:9" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C21" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="E21" s="4" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="E22" s="14" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="C23" s="14" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="D29" s="24"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C24" s="14" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D29" s="22"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1524,123 +1555,123 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView zoomScale="226" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.33203125" style="25" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9" style="25"/>
-    <col min="3" max="3" width="12.5" style="25" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.1640625" style="26" customWidth="1"/>
-    <col min="5" max="5" width="18.6640625" style="25" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="9" style="25"/>
+    <col min="1" max="1" width="13.375" style="23" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9" style="23"/>
+    <col min="3" max="3" width="12.5" style="23" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.125" style="24" customWidth="1"/>
+    <col min="5" max="5" width="18.625" style="23" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9" style="23"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A1" s="25" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="23" t="s">
+        <v>51</v>
+      </c>
+      <c r="B1" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="C1" s="23" t="s">
+        <v>52</v>
+      </c>
+      <c r="D1" s="24" t="s">
+        <v>64</v>
+      </c>
+      <c r="E1" s="23" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A2" s="23" t="s">
+        <v>59</v>
+      </c>
+      <c r="B2" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="C2" s="25">
+        <v>42300</v>
+      </c>
+      <c r="D2" s="26" t="s">
+        <v>65</v>
+      </c>
+      <c r="E2" s="27" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="23" t="s">
+        <v>59</v>
+      </c>
+      <c r="B3" s="23" t="s">
+        <v>57</v>
+      </c>
+      <c r="C3" s="25">
+        <v>42300</v>
+      </c>
+      <c r="E3" s="27" t="s">
         <v>58</v>
       </c>
-      <c r="B1" s="25" t="s">
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="B4" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="C4" s="25">
+        <v>42300</v>
+      </c>
+      <c r="E4" s="27" t="s">
         <v>62</v>
       </c>
-      <c r="C1" s="25" t="s">
-        <v>59</v>
-      </c>
-      <c r="D1" s="26" t="s">
-        <v>71</v>
-      </c>
-      <c r="E1" s="25" t="s">
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="23" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" ht="51" x14ac:dyDescent="0.2">
-      <c r="A2" s="25" t="s">
+      <c r="C5" s="25">
+        <v>42300</v>
+      </c>
+      <c r="E5" s="27" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="23" t="s">
         <v>66</v>
       </c>
-      <c r="B2" s="25" t="s">
-        <v>63</v>
-      </c>
-      <c r="C2" s="27">
+      <c r="C6" s="25">
         <v>42300</v>
       </c>
-      <c r="D2" s="28" t="s">
-        <v>72</v>
-      </c>
-      <c r="E2" s="29" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="25" t="s">
+      <c r="E6" s="22" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="23" t="s">
         <v>66</v>
       </c>
-      <c r="B3" s="25" t="s">
-        <v>64</v>
-      </c>
-      <c r="C3" s="27">
+      <c r="C7" s="25">
         <v>42300</v>
       </c>
-      <c r="E3" s="29" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="25" t="s">
+      <c r="E7" s="27" t="s">
         <v>67</v>
       </c>
-      <c r="B4" s="25" t="s">
-        <v>68</v>
-      </c>
-      <c r="C4" s="27">
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="23" t="s">
+        <v>66</v>
+      </c>
+      <c r="C8" s="25">
         <v>42300</v>
       </c>
-      <c r="E4" s="29" t="s">
+      <c r="E8" s="27" t="s">
         <v>69</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="25" t="s">
-        <v>67</v>
-      </c>
-      <c r="C5" s="27">
-        <v>42300</v>
-      </c>
-      <c r="E5" s="29" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="25" t="s">
-        <v>73</v>
-      </c>
-      <c r="C6" s="27">
-        <v>42300</v>
-      </c>
-      <c r="E6" s="24" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="25" t="s">
-        <v>73</v>
-      </c>
-      <c r="C7" s="27">
-        <v>42300</v>
-      </c>
-      <c r="E7" s="29" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="25" t="s">
-        <v>73</v>
-      </c>
-      <c r="C8" s="27">
-        <v>42300</v>
-      </c>
-      <c r="E8" s="29" t="s">
-        <v>76</v>
       </c>
     </row>
   </sheetData>

</xml_diff>